<commit_message>
Didn't actually update this...
</commit_message>
<xml_diff>
--- a/src/com/domo/featurebuilder/resources/domoWebEndpoints.xlsx
+++ b/src/com/domo/featurebuilder/resources/domoWebEndpoints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="domoWebEndpoints.csv" sheetId="1" r:id="rId1"/>
@@ -1069,8 +1069,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1098,7 +1110,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1109,6 +1121,12 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1119,6 +1137,12 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -1496,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>